<commit_message>
Mainform config persistence/ui theme persistence.
</commit_message>
<xml_diff>
--- a/Data/UI Map Data.xlsx
+++ b/Data/UI Map Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\App Frameworks\DevExpress MDI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A970F698-7EF0-4B81-BD89-C699D1FE6795}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2B994A-6624-495F-8220-B6300DD13059}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="8475" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{C92C9229-1C66-49D2-84EB-B6B284FB8570}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="119">
   <si>
     <t>Basic</t>
   </si>
@@ -399,6 +399,9 @@
   </si>
   <si>
     <t>DocWinIcon</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -4985,7 +4988,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:F1"/>
+      <selection pane="topRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5041,8 +5044,12 @@
       <c r="D4" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
@@ -5057,8 +5064,12 @@
       <c r="D5" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="E5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -5073,8 +5084,12 @@
       <c r="D6" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
@@ -5089,8 +5104,12 @@
       <c r="D7" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -5105,8 +5124,12 @@
       <c r="D8" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="E8" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
@@ -5121,8 +5144,12 @@
       <c r="D9" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -5137,8 +5164,12 @@
       <c r="D10" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="E10" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
@@ -5153,8 +5184,12 @@
       <c r="D11" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -5169,8 +5204,12 @@
       <c r="D12" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">

</xml_diff>